<commit_message>
Adding tester row to excel documents
</commit_message>
<xml_diff>
--- a/A_Yellow Enemy.xlsx
+++ b/A_Yellow Enemy.xlsx
@@ -12,29 +12,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Test ID</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>A01</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>User Stories</t>
   </si>
   <si>
+    <t>As an expert gamer, I would like to be able to survive against the yellow enemy so that I can improve my score.</t>
+  </si>
+  <si>
     <t>Test Owner</t>
   </si>
   <si>
-    <t>As an expert gamer, I would like to be able to survive against the yellow enemy so that I can improve my score.</t>
-  </si>
-  <si>
     <t>Timothy Carta</t>
   </si>
   <si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Checks to see if the player can successfully survive against "yellow enemy"</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
   <si>
     <t>Procedure</t>
@@ -114,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -130,6 +133,10 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -189,30 +196,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -224,6 +231,9 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -472,20 +482,20 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
@@ -493,26 +503,26 @@
     </row>
     <row r="3">
       <c r="A3" s="12"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -539,28 +549,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="11"/>
     </row>
     <row r="3">
@@ -568,19 +578,19 @@
         <v>9</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
       <c r="F3" s="11"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5">
@@ -590,105 +600,115 @@
       <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="20"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="18">
-        <v>2.0</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="18">
+      <c r="A10" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="19">
         <v>3.0</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="22">
+      <c r="C11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="23">
         <v>4.0</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="24" t="s">
+      <c r="C12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>